<commit_message>
Amended ExtractCVs.xaml file to change %CVMatch variable to integer type
</commit_message>
<xml_diff>
--- a/Output/Output_IT_CVs - Copy.xlsx
+++ b/Output/Output_IT_CVs - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAJ01_JobMatchingForPlacements\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F6E20E-1DFB-4C29-9F0B-239D33E803B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA5198-48CE-48DF-B0D9-A57B16EB8492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{34DDD9C4-B25B-4E4D-8771-E8077D4555D8}"/>
   </bookViews>
@@ -463,8 +463,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -500,7 +500,7 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>40.54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.75">
@@ -514,7 +514,7 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>40.54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.75">
@@ -528,7 +528,7 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>35.14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.75">
@@ -542,7 +542,7 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>35.14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.75">
@@ -556,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>29.73</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.75">
@@ -570,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>18.920000000000002</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.75">
@@ -584,7 +584,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>13.51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.75">
@@ -598,7 +598,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>13.51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.75">
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.75">
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.75">
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.75">
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.75">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.75">
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>